<commit_message>
modify Adm. Tribunales databases to have same Regiones for all years
</commit_message>
<xml_diff>
--- a/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
+++ b/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlando.hernandez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DEBF692-8B97-4540-8DFB-6E74B8E7F646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB155DD7-AAFC-4703-BA1A-42636C086389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7845" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7845" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2021" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
   <si>
     <t>Región</t>
   </si>
@@ -56,6 +56,9 @@
     <t>Adjuntas</t>
   </si>
   <si>
+    <t>Aguadilla</t>
+  </si>
+  <si>
     <t>Aibonito</t>
   </si>
   <si>
@@ -71,53 +74,47 @@
     <t>Carolina</t>
   </si>
   <si>
+    <t>Fajardo</t>
+  </si>
+  <si>
+    <t>Guayama</t>
+  </si>
+  <si>
     <t>Guaynabo</t>
   </si>
   <si>
+    <t>Humacao</t>
+  </si>
+  <si>
+    <t>Mayagüez</t>
+  </si>
+  <si>
+    <t>Ponce</t>
+  </si>
+  <si>
+    <t>San Juan</t>
+  </si>
+  <si>
     <t>Utuado</t>
   </si>
   <si>
+    <t>No indica</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bayamón </t>
   </si>
   <si>
-    <t>Fajardo</t>
-  </si>
-  <si>
     <t xml:space="preserve">San Juan </t>
   </si>
   <si>
-    <t>No indica</t>
-  </si>
-  <si>
-    <t>Aguadilla</t>
-  </si>
-  <si>
     <t xml:space="preserve">Caguas </t>
-  </si>
-  <si>
-    <t>Guayama</t>
-  </si>
-  <si>
-    <t>Humacao</t>
-  </si>
-  <si>
-    <t>Mayaguez</t>
-  </si>
-  <si>
-    <t>Ponce</t>
-  </si>
-  <si>
-    <t>San Juan</t>
-  </si>
-  <si>
-    <t>Bayamon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +122,12 @@
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,9 +150,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,153 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1">
-        <f>SUM(B2:B9)</f>
-        <v>11</v>
-      </c>
-      <c r="C10" s="1">
-        <f t="shared" ref="C10:D10" si="0">SUM(C2:C9)</f>
-        <v>4</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A17" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -602,87 +463,170 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <f>SUM(B2:B7)</f>
         <v>10</v>
       </c>
-      <c r="C8">
-        <f>SUM(C2:C7)</f>
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <f>SUM(D2:D7)</f>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <f>SUM(B2:B16)</f>
+        <v>11</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" ref="C18:D18" si="0">SUM(C2:C16)</f>
+        <v>4</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -691,15 +635,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:D15"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -725,33 +666,48 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -761,72 +717,113 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B15">
-        <f>SUM(B2:B14)</f>
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <f t="shared" ref="C15:D15" si="0">SUM(C2:C14)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B4:B17)</f>
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <f>SUM(C4:C17)</f>
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <f>SUM(D4:D17)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D9"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -851,100 +848,306 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B3:B16)</f>
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:D18" si="0">SUM(C3:C16)</f>
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A40" sqref="A23:A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
       </c>
       <c r="B9">
-        <f>SUM(B2:B8)</f>
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="C9">
-        <f t="shared" ref="C9:D9" si="0">SUM(C2:C8)</f>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B5:B16)</f>
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:D18" si="0">SUM(C5:C16)</f>
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add modifications made by Dra. Idania
</commit_message>
<xml_diff>
--- a/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
+++ b/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlando.hernandez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB155DD7-AAFC-4703-BA1A-42636C086389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{12ED7658-C94E-4A42-B068-30AC5D8474BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7845" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7845" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2021" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="21">
   <si>
     <t>Región</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Otra razón</t>
   </si>
   <si>
-    <t>Adjuntas</t>
-  </si>
-  <si>
     <t>Aguadilla</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
   </si>
   <si>
     <t>Guayama</t>
-  </si>
-  <si>
-    <t>Guaynabo</t>
   </si>
   <si>
     <t>Humacao</t>
@@ -434,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A2:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -462,32 +456,32 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -495,7 +489,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -506,12 +503,9 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
         <v>1</v>
       </c>
     </row>
@@ -520,28 +514,25 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1"/>
@@ -553,19 +544,14 @@
         <v>12</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
@@ -575,7 +561,7 @@
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1"/>
@@ -585,11 +571,18 @@
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="1"/>
@@ -597,36 +590,18 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <f>SUM(B2:B14)</f>
+        <v>11</v>
+      </c>
+      <c r="C16" s="1">
+        <f>SUM(C2:C14)</f>
+        <v>4</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1">
-        <f>SUM(B2:B16)</f>
-        <v>11</v>
-      </c>
-      <c r="C18" s="1">
-        <f t="shared" ref="C18:D18" si="0">SUM(C2:C16)</f>
-        <v>4</v>
-      </c>
-      <c r="D18" s="1">
-        <f t="shared" si="0"/>
+        <f>SUM(D2:D14)</f>
         <v>7</v>
       </c>
     </row>
@@ -637,10 +612,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -665,13 +640,19 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -681,33 +662,27 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -719,17 +694,17 @@
       <c r="A8" t="s">
         <v>10</v>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -748,7 +723,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -758,7 +739,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -769,45 +750,29 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <f>SUM(B4:B17)</f>
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <f>SUM(B3:B15)</f>
         <v>10</v>
       </c>
-      <c r="C18">
-        <f>SUM(C4:C17)</f>
+      <c r="C16">
+        <f>SUM(C3:C15)</f>
         <v>3</v>
       </c>
-      <c r="D18">
-        <f>SUM(D4:D17)</f>
+      <c r="D16">
+        <f>SUM(D3:D15)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="2"/>
+    <row r="22" spans="1:1">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -819,10 +784,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -855,21 +820,21 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -879,7 +844,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -901,6 +866,12 @@
       <c r="A11" t="s">
         <v>13</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
@@ -911,12 +882,6 @@
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
@@ -930,39 +895,29 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <f>SUM(B3:B16)</f>
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <f t="shared" ref="C18:D18" si="0">SUM(C3:C16)</f>
-        <v>2</v>
-      </c>
-      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <f>SUM(B2:B14)</f>
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:D16" si="0">SUM(C2:C14)</f>
+        <v>2</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="2"/>
+    <row r="22" spans="1:1">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -971,10 +926,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A40" sqref="A23:A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -999,12 +954,12 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1012,16 +967,25 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1029,52 +993,43 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
@@ -1085,9 +1040,15 @@
       <c r="A12" t="s">
         <v>14</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1098,56 +1059,40 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <f>SUM(B4:B14)</f>
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:D16" si="0">SUM(C4:C14)</f>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <f>SUM(B5:B16)</f>
-        <v>13</v>
-      </c>
-      <c r="C18">
-        <f t="shared" ref="C18:D18" si="0">SUM(C5:C16)</f>
-        <v>3</v>
-      </c>
-      <c r="D18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="2"/>
+    <row r="22" spans="1:1">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new data for Adm. Tribunales
</commit_message>
<xml_diff>
--- a/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
+++ b/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28813"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlando.hernandez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6454909D-E86F-4A5A-9816-49A1D68A5FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08D990F9-D599-41F4-AFC7-1BA277ED777E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7845" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7845" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2021" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="22">
   <si>
     <t>Región</t>
   </si>
@@ -103,13 +103,16 @@
   </si>
   <si>
     <t xml:space="preserve">Caguas </t>
+  </si>
+  <si>
+    <t>Mayaguez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +125,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -145,10 +155,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,8 +798,8 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -799,99 +810,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>17</v>
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -900,15 +977,15 @@
       </c>
       <c r="B16">
         <f>SUM(B2:B14)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <f t="shared" ref="C16:D16" si="0">SUM(C2:C14)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:1">
@@ -1104,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37247A8D-E653-4823-BD28-94768F3C7E21}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modify in Adm. Tribunales data with Mayaguez wrong
</commit_message>
<xml_diff>
--- a/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
+++ b/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlando.hernandez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\administracion_de_tribunales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08D990F9-D599-41F4-AFC7-1BA277ED777E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77F8698-FAA9-4A14-8356-19C05A527476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7845" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2021" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="21">
   <si>
     <t>Región</t>
   </si>
@@ -103,16 +103,13 @@
   </si>
   <si>
     <t xml:space="preserve">Caguas </t>
-  </si>
-  <si>
-    <t>Mayaguez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,14 +443,14 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,14 +464,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -485,7 +482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -496,7 +493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -510,7 +507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -521,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -535,7 +532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -543,7 +540,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -551,35 +548,35 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -593,14 +590,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -630,14 +627,14 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -651,12 +648,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -667,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -678,7 +675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -692,17 +689,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -713,27 +710,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -744,12 +741,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -760,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -777,13 +774,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
     </row>
   </sheetData>
@@ -798,18 +795,18 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -823,7 +820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -835,7 +832,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -847,7 +844,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -855,7 +852,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -867,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -875,7 +872,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -883,7 +880,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -891,7 +888,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -903,7 +900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -911,9 +908,9 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -925,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -933,7 +930,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -945,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
@@ -957,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -971,7 +968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -988,13 +985,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
     </row>
   </sheetData>
@@ -1007,17 +1004,17 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="A1:D16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1031,17 +1028,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1052,7 +1049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1066,7 +1063,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1077,12 +1074,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1093,7 +1090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1104,17 +1101,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1125,12 +1122,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1141,12 +1138,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1163,13 +1160,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
     </row>
   </sheetData>
@@ -1181,13 +1178,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37247A8D-E653-4823-BD28-94768F3C7E21}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1201,62 +1198,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1267,17 +1264,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
modify data in excel for Administracion de Tribunales
</commit_message>
<xml_diff>
--- a/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
+++ b/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\administracion_de_tribunales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77F8698-FAA9-4A14-8356-19C05A527476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B20178D-6168-44F2-B0D2-9D08BC237FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2021" sheetId="5" r:id="rId1"/>
@@ -122,7 +122,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,7 +1179,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1278,6 +1278,18 @@
       <c r="A16" t="s">
         <v>1</v>
       </c>
+      <c r="B16">
+        <f>SUM(B2:B15)</f>
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:D16" si="0">SUM(C2:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify drcCasosInv.xlsx to add data 0's for 2024, modify plots in Tribunales to have y-axis with whole numbers and modify upper_y_lim in utils.R
</commit_message>
<xml_diff>
--- a/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
+++ b/data/administracion_de_tribunales/OP_LEY148Archivadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\administracion_de_tribunales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B20178D-6168-44F2-B0D2-9D08BC237FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6164E3-32BF-4FF2-B0AE-B68DF00C0922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2021" sheetId="5" r:id="rId1"/>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,7 +624,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37247A8D-E653-4823-BD28-94768F3C7E21}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>